<commit_message>
Added elec calibration info to calibrated specs
</commit_message>
<xml_diff>
--- a/test/test_data/dj-specs-test.xlsx
+++ b/test/test_data/dj-specs-test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="31455" windowHeight="10515" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="470" windowWidth="31460" windowHeight="10520" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioInfo" sheetId="1" r:id="rId1"/>
@@ -525,20 +525,20 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.1796875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" customWidth="1"/>
-    <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -567,7 +567,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -609,19 +609,19 @@
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>9</v>
       </c>
@@ -656,7 +656,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -694,7 +694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -732,7 +732,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -760,48 +760,48 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD2"/>
+  <dimension ref="A1:X2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AC12" sqref="AC12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="22.1796875" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="40.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.140625" style="2" customWidth="1"/>
-    <col min="24" max="24" width="12.7109375" style="2" customWidth="1"/>
-    <col min="25" max="25" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26.81640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="40.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.453125" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.1796875" style="2" customWidth="1"/>
+    <col min="24" max="24" width="12.7265625" style="2" customWidth="1"/>
+    <col min="25" max="25" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.26953125" style="2" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.1796875" style="2" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
     <col min="29" max="30" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="50" width="9.140625" style="2" customWidth="1"/>
-    <col min="51" max="16384" width="9.140625" style="2"/>
+    <col min="31" max="50" width="9.1796875" style="2" customWidth="1"/>
+    <col min="51" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>20</v>
       </c>
@@ -874,14 +874,8 @@
       <c r="X1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
-      <c r="AB1" s="1"/>
-      <c r="AC1" s="1"/>
-      <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Updated to work with flexible years and technologies
</commit_message>
<xml_diff>
--- a/test/test_data/dj-specs-test.xlsx
+++ b/test/test_data/dj-specs-test.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="470" windowWidth="31460" windowHeight="10520" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="31455" windowHeight="10515" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ScenarioInfo" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Scenario</t>
   </si>
@@ -32,9 +32,6 @@
     <t>Target_electricity_consumption_level</t>
   </si>
   <si>
-    <t>Electrification_target_5_years</t>
-  </si>
-  <si>
     <t>Grid_electricity_generation_cost</t>
   </si>
   <si>
@@ -92,9 +89,6 @@
     <t>StartYear</t>
   </si>
   <si>
-    <t>EndYEar</t>
-  </si>
-  <si>
     <t>PopStartYear</t>
   </si>
   <si>
@@ -156,6 +150,15 @@
   </si>
   <si>
     <t>dj</t>
+  </si>
+  <si>
+    <t>ElecTarget</t>
+  </si>
+  <si>
+    <t>EndYear</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -198,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -221,12 +224,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -238,6 +252,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,26 +536,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
-    <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -563,11 +579,8 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -581,7 +594,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -590,9 +603,6 @@
         <v>0</v>
       </c>
       <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
         <v>0</v>
       </c>
     </row>
@@ -603,36 +613,38 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.81640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.453125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
-      </c>
-      <c r="E1" t="s">
-        <v>12</v>
       </c>
       <c r="F1" t="s">
         <v>13</v>
@@ -652,11 +664,8 @@
       <c r="K1" t="s">
         <v>18</v>
       </c>
-      <c r="L1" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -672,29 +681,26 @@
       <c r="E2" s="4">
         <v>0.83333333330000003</v>
       </c>
-      <c r="F2">
-        <v>9999</v>
-      </c>
-      <c r="G2" s="4">
+      <c r="F2" s="4">
         <v>2.4E-2</v>
       </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
       <c r="H2">
-        <v>1</v>
+        <v>99</v>
       </c>
       <c r="I2">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="J2">
+        <v>5</v>
+      </c>
+      <c r="K2">
         <v>0</v>
       </c>
-      <c r="K2">
-        <v>5</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -711,28 +717,25 @@
         <v>0.83333333330000003</v>
       </c>
       <c r="F3" s="4">
-        <v>3.5875798059999999</v>
-      </c>
-      <c r="G3" s="4">
         <v>0.03</v>
       </c>
+      <c r="G3">
+        <v>1.25</v>
+      </c>
       <c r="H3">
-        <v>1.25</v>
+        <v>99</v>
       </c>
       <c r="I3">
-        <v>99</v>
+        <v>0</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K3">
-        <v>4</v>
-      </c>
-      <c r="L3">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -742,13 +745,13 @@
       <c r="D4">
         <v>6</v>
       </c>
-      <c r="H4">
+      <c r="G4">
         <v>0.75</v>
       </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
       <c r="K4">
-        <v>4</v>
-      </c>
-      <c r="L4">
         <v>2</v>
       </c>
     </row>
@@ -760,177 +763,263 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X2"/>
+  <dimension ref="A1:AA3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AC12" sqref="AC12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="8.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="22.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="23" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="26.81640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="40.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.453125" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="12.1796875" style="2" customWidth="1"/>
-    <col min="24" max="24" width="12.7265625" style="2" customWidth="1"/>
-    <col min="25" max="25" width="14.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="29" max="30" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="31" max="50" width="9.1796875" style="2" customWidth="1"/>
-    <col min="51" max="16384" width="9.1796875" style="2"/>
+    <col min="1" max="2" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.85546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="23" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="20.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="40.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.140625" style="2" customWidth="1"/>
+    <col min="27" max="27" width="12.7109375" style="2" customWidth="1"/>
+    <col min="28" max="28" width="14.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="12.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="34" max="53" width="9.140625" style="2" customWidth="1"/>
+    <col min="54" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="K1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="W1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>2025</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="D2" s="2">
+        <v>2018</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2030</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0.83333333330000003</v>
+      </c>
+      <c r="G2" s="2">
+        <v>971000</v>
+      </c>
+      <c r="H2" s="2">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="K2" s="2">
+        <v>1179150</v>
+      </c>
+      <c r="L2" s="4">
+        <v>3.5875798059999999</v>
+      </c>
+      <c r="M2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="N2" s="2">
+        <v>7.7</v>
+      </c>
+      <c r="O2" s="2">
+        <v>6.5</v>
+      </c>
+      <c r="P2" s="2">
+        <v>4426</v>
+      </c>
+      <c r="Q2" s="2">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="R2" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="S2" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="T2" s="2">
+        <v>50</v>
+      </c>
+      <c r="U2" s="2">
+        <v>19</v>
+      </c>
+      <c r="V2" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="W2" s="2">
+        <v>0.26</v>
+      </c>
+      <c r="X2" s="2">
+        <v>0.7</v>
+      </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="2">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2030</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="2">
         <v>2018</v>
       </c>
-      <c r="D2" s="2">
+      <c r="E3" s="2">
         <v>2030</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2">
         <v>971000</v>
       </c>
-      <c r="F2" s="2">
+      <c r="H3" s="2">
         <v>0.77800000000000002</v>
       </c>
-      <c r="I2" s="2">
+      <c r="K3" s="2">
         <v>1179150</v>
       </c>
-      <c r="J2" s="2">
+      <c r="L3" s="2">
+        <v>99999999</v>
+      </c>
+      <c r="M3" s="2">
         <v>0.8</v>
       </c>
-      <c r="K2" s="2">
+      <c r="N3" s="2">
         <v>7.7</v>
       </c>
-      <c r="L2" s="2">
+      <c r="O3" s="2">
         <v>6.5</v>
       </c>
-      <c r="M2" s="2">
+      <c r="P3" s="2">
         <v>4426</v>
       </c>
-      <c r="N2" s="2">
+      <c r="Q3" s="2">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="O2" s="2">
+      <c r="R3" s="2">
         <v>0.8</v>
       </c>
-      <c r="P2" s="2">
+      <c r="S3" s="2">
         <v>0.1</v>
       </c>
-      <c r="Q2" s="2">
+      <c r="T3" s="2">
         <v>50</v>
       </c>
-      <c r="R2" s="2">
+      <c r="U3" s="2">
         <v>19</v>
       </c>
-      <c r="S2" s="2">
+      <c r="V3" s="2">
         <v>0.6</v>
       </c>
-      <c r="T2" s="2">
+      <c r="W3" s="2">
         <v>0.26</v>
       </c>
-      <c r="U2" s="2">
+      <c r="X3" s="2">
         <v>0.7</v>
       </c>
     </row>

</xml_diff>